<commit_message>
ready for deploy v1
</commit_message>
<xml_diff>
--- a/resources/EEE -211_Marks_2019.xlsx
+++ b/resources/EEE -211_Marks_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/All-from 2019/Question Setter/2nd Semester Question and Marks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhidwan/Desktop/Academic project/srps/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FC909A-894D-8242-A316-4331E24A6B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED20453-60AE-444A-A691-72CB04EAC6B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$97</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -305,7 +296,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -343,6 +334,11 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -364,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -763,41 +759,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -892,9 +858,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -904,9 +867,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,9 +888,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -970,12 +927,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1003,6 +960,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1030,18 +990,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,20 +1403,20 @@
   </sheetPr>
   <dimension ref="A1:AB90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="28" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="28" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="38" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" style="28" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="40" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="38" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="28" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="38" customWidth="1"/>
     <col min="9" max="10" width="6.6640625" style="28" customWidth="1"/>
     <col min="11" max="11" width="13.1640625" style="28" customWidth="1"/>
     <col min="12" max="17" width="11.5" style="28" customWidth="1"/>
@@ -1477,19 +1426,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="27"/>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
@@ -1509,19 +1458,19 @@
       <c r="AB1" s="27"/>
     </row>
     <row r="2" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
@@ -1541,19 +1490,19 @@
       <c r="AB2" s="27"/>
     </row>
     <row r="3" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
       <c r="N3" s="27"/>
@@ -1573,19 +1522,19 @@
       <c r="AB3" s="27"/>
     </row>
     <row r="4" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
       <c r="L4" s="27"/>
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
@@ -1605,19 +1554,19 @@
       <c r="AB4" s="27"/>
     </row>
     <row r="5" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
       <c r="L5" s="27"/>
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
@@ -1667,23 +1616,23 @@
       <c r="AB6" s="27"/>
     </row>
     <row r="7" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="63" t="s">
+      <c r="A7" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="65" t="s">
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="62" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="27"/>
@@ -1705,22 +1654,22 @@
       <c r="AB7" s="27"/>
     </row>
     <row r="8" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="66"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="63"/>
     </row>
     <row r="9" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="67"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="50">
+      <c r="A9" s="64"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="47">
         <v>1</v>
       </c>
       <c r="D9" s="30">
@@ -1741,1574 +1690,1706 @@
       <c r="I9" s="31">
         <v>7</v>
       </c>
-      <c r="J9" s="51">
-        <v>8</v>
-      </c>
-      <c r="K9" s="67"/>
-    </row>
-    <row r="10" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="32"/>
-      <c r="B10" s="53" t="s">
+      <c r="J9" s="48">
+        <v>8</v>
+      </c>
+      <c r="K9" s="64"/>
+    </row>
+    <row r="10" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="76">
+        <v>19702001</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="44">
         <v>4</v>
       </c>
-      <c r="D10" s="34">
-        <v>7</v>
-      </c>
-      <c r="E10" s="33">
-        <v>8</v>
-      </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="55">
+      <c r="D10" s="33">
+        <v>7</v>
+      </c>
+      <c r="E10" s="32">
+        <v>8</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="52">
         <f t="shared" ref="K10:K29" si="0">SUM(C10,D10,E10,F10,G10,H10,I10,J10)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="54" t="s">
+    <row r="11" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="76">
+        <v>19702003</v>
+      </c>
+      <c r="B11" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="48">
-        <v>6</v>
-      </c>
-      <c r="D11" s="38">
-        <v>8</v>
-      </c>
-      <c r="E11" s="37">
-        <v>8</v>
-      </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="56">
+      <c r="C11" s="45">
+        <v>6</v>
+      </c>
+      <c r="D11" s="36">
+        <v>8</v>
+      </c>
+      <c r="E11" s="35">
+        <v>8</v>
+      </c>
+      <c r="F11" s="36"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="36"/>
-      <c r="B12" s="53" t="s">
+    <row r="12" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="76">
+        <v>19702004</v>
+      </c>
+      <c r="B12" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="38">
-        <v>7</v>
-      </c>
-      <c r="E12" s="37">
-        <v>8</v>
-      </c>
-      <c r="F12" s="38">
-        <v>8</v>
-      </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="56">
+      <c r="C12" s="45"/>
+      <c r="D12" s="36">
+        <v>7</v>
+      </c>
+      <c r="E12" s="35">
+        <v>8</v>
+      </c>
+      <c r="F12" s="36">
+        <v>8</v>
+      </c>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="53">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
-      <c r="B13" s="54" t="s">
+    <row r="13" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="76">
+        <v>19702005</v>
+      </c>
+      <c r="B13" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="48">
-        <v>6</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="37">
-        <v>8</v>
-      </c>
-      <c r="F13" s="38">
-        <v>8</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="56">
+      <c r="C13" s="45">
+        <v>6</v>
+      </c>
+      <c r="D13" s="36"/>
+      <c r="E13" s="35">
+        <v>8</v>
+      </c>
+      <c r="F13" s="36">
+        <v>8</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="36"/>
-      <c r="B14" s="53" t="s">
+    <row r="14" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="76">
+        <v>19702006</v>
+      </c>
+      <c r="B14" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="48">
-        <v>8</v>
-      </c>
-      <c r="D14" s="38">
-        <v>8</v>
-      </c>
-      <c r="E14" s="37">
-        <v>8</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="56">
+      <c r="C14" s="45">
+        <v>8</v>
+      </c>
+      <c r="D14" s="36">
+        <v>8</v>
+      </c>
+      <c r="E14" s="35">
+        <v>8</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="53">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="54" t="s">
+    <row r="15" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="76">
+        <v>19702007</v>
+      </c>
+      <c r="B15" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="48">
-        <v>6</v>
-      </c>
-      <c r="D15" s="38">
-        <v>8</v>
-      </c>
-      <c r="E15" s="37">
-        <v>8</v>
-      </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="56">
+      <c r="C15" s="45">
+        <v>6</v>
+      </c>
+      <c r="D15" s="36">
+        <v>8</v>
+      </c>
+      <c r="E15" s="35">
+        <v>8</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="36"/>
-      <c r="B16" s="53" t="s">
+    <row r="16" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="76">
+        <v>19702008</v>
+      </c>
+      <c r="B16" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="38">
-        <v>8</v>
-      </c>
-      <c r="E16" s="37">
-        <v>7</v>
-      </c>
-      <c r="F16" s="38">
-        <v>8</v>
-      </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="56">
+      <c r="C16" s="45"/>
+      <c r="D16" s="36">
+        <v>8</v>
+      </c>
+      <c r="E16" s="35">
+        <v>7</v>
+      </c>
+      <c r="F16" s="36">
+        <v>8</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="53">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="54" t="s">
+    <row r="17" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="76">
+        <v>19702009</v>
+      </c>
+      <c r="B17" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="38">
-        <v>8</v>
-      </c>
-      <c r="E17" s="37">
-        <v>7</v>
-      </c>
-      <c r="F17" s="38">
+      <c r="C17" s="45"/>
+      <c r="D17" s="36">
+        <v>8</v>
+      </c>
+      <c r="E17" s="35">
+        <v>7</v>
+      </c>
+      <c r="F17" s="36">
         <v>8</v>
       </c>
       <c r="G17" s="27"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="56">
+      <c r="H17" s="36"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="53">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="36"/>
-      <c r="B18" s="53" t="s">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="76">
+        <v>19702010</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="48">
-        <v>6</v>
-      </c>
-      <c r="D18" s="38">
-        <v>8</v>
-      </c>
-      <c r="E18" s="37">
-        <v>8</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="56">
+      <c r="C18" s="45">
+        <v>6</v>
+      </c>
+      <c r="D18" s="36">
+        <v>8</v>
+      </c>
+      <c r="E18" s="35">
+        <v>8</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="54" t="s">
+    <row r="19" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="76">
+        <v>19702011</v>
+      </c>
+      <c r="B19" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="45">
         <v>4</v>
       </c>
-      <c r="D19" s="38">
-        <v>8</v>
-      </c>
-      <c r="E19" s="37">
-        <v>8</v>
-      </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="56">
+      <c r="D19" s="36">
+        <v>8</v>
+      </c>
+      <c r="E19" s="35">
+        <v>8</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="53">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="36"/>
-      <c r="B20" s="53" t="s">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="76">
+        <v>19702012</v>
+      </c>
+      <c r="B20" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="48">
-        <v>6</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="37">
-        <v>7</v>
-      </c>
-      <c r="F20" s="38">
-        <v>8</v>
-      </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="56">
+      <c r="C20" s="45">
+        <v>6</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="35">
+        <v>7</v>
+      </c>
+      <c r="F20" s="36">
+        <v>8</v>
+      </c>
+      <c r="G20" s="35"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="53">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="54" t="s">
+    <row r="21" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="76">
+        <v>19702015</v>
+      </c>
+      <c r="B21" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="38">
-        <v>7</v>
-      </c>
-      <c r="E21" s="37">
-        <v>7</v>
-      </c>
-      <c r="F21" s="38">
+      <c r="C21" s="45"/>
+      <c r="D21" s="36">
+        <v>7</v>
+      </c>
+      <c r="E21" s="35">
+        <v>7</v>
+      </c>
+      <c r="F21" s="36">
         <v>4</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="56">
+      <c r="G21" s="35"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="53">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="36"/>
-      <c r="B22" s="53" t="s">
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="76">
+        <v>19702016</v>
+      </c>
+      <c r="B22" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="38">
-        <v>8</v>
-      </c>
-      <c r="E22" s="37">
-        <v>7</v>
-      </c>
-      <c r="F22" s="38">
-        <v>8</v>
-      </c>
-      <c r="G22" s="37"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="36">
+        <v>8</v>
+      </c>
+      <c r="E22" s="35">
+        <v>7</v>
+      </c>
+      <c r="F22" s="36">
+        <v>8</v>
+      </c>
+      <c r="G22" s="35"/>
       <c r="H22" s="29"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="56">
+      <c r="I22" s="35"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="53">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36"/>
-      <c r="B23" s="54" t="s">
+    <row r="23" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="76">
+        <v>19702017</v>
+      </c>
+      <c r="B23" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="38">
-        <v>7</v>
-      </c>
-      <c r="E23" s="37">
-        <v>8</v>
-      </c>
-      <c r="F23" s="38">
-        <v>8</v>
-      </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="56">
+      <c r="C23" s="45"/>
+      <c r="D23" s="36">
+        <v>7</v>
+      </c>
+      <c r="E23" s="35">
+        <v>8</v>
+      </c>
+      <c r="F23" s="36">
+        <v>8</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="53">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="36"/>
-      <c r="B24" s="53" t="s">
+    <row r="24" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="76">
+        <v>19702018</v>
+      </c>
+      <c r="B24" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="48">
-        <v>6</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="37">
-        <v>8</v>
-      </c>
-      <c r="F24" s="38">
-        <v>7</v>
-      </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="56">
+      <c r="C24" s="45">
+        <v>6</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="35">
+        <v>8</v>
+      </c>
+      <c r="F24" s="36">
+        <v>7</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="53">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="B25" s="54" t="s">
+    <row r="25" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="76">
+        <v>19702019</v>
+      </c>
+      <c r="B25" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="45">
         <v>3</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="36">
         <v>5</v>
       </c>
-      <c r="E25" s="37">
-        <v>6</v>
-      </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="56">
+      <c r="E25" s="35">
+        <v>6</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="53">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="36"/>
-      <c r="B26" s="53" t="s">
+    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="76">
+        <v>19702020</v>
+      </c>
+      <c r="B26" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="48">
-        <v>6</v>
-      </c>
-      <c r="D26" s="38">
-        <v>7</v>
-      </c>
-      <c r="E26" s="37">
-        <v>7</v>
-      </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="56">
+      <c r="C26" s="45">
+        <v>6</v>
+      </c>
+      <c r="D26" s="36">
+        <v>7</v>
+      </c>
+      <c r="E26" s="35">
+        <v>7</v>
+      </c>
+      <c r="F26" s="36"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="53">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="54" t="s">
+    <row r="27" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="76">
+        <v>19702021</v>
+      </c>
+      <c r="B27" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="38">
-        <v>7</v>
-      </c>
-      <c r="E27" s="37">
-        <v>7</v>
-      </c>
-      <c r="F27" s="38">
-        <v>7</v>
-      </c>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="56">
+      <c r="C27" s="45"/>
+      <c r="D27" s="36">
+        <v>7</v>
+      </c>
+      <c r="E27" s="35">
+        <v>7</v>
+      </c>
+      <c r="F27" s="36">
+        <v>7</v>
+      </c>
+      <c r="G27" s="35"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="53">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="36"/>
-      <c r="B28" s="53" t="s">
+    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="76">
+        <v>19702022</v>
+      </c>
+      <c r="B28" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="42">
-        <v>7</v>
-      </c>
-      <c r="E28" s="41">
-        <v>6</v>
-      </c>
-      <c r="F28" s="38">
-        <v>7</v>
-      </c>
-      <c r="G28" s="41"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="56">
+      <c r="C28" s="46"/>
+      <c r="D28" s="40">
+        <v>7</v>
+      </c>
+      <c r="E28" s="39">
+        <v>6</v>
+      </c>
+      <c r="F28" s="36">
+        <v>7</v>
+      </c>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="53">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="54" t="s">
+    <row r="29" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="76">
+        <v>19702023</v>
+      </c>
+      <c r="B29" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="42">
-        <v>6</v>
-      </c>
-      <c r="E29" s="41">
-        <v>8</v>
-      </c>
-      <c r="F29" s="38">
-        <v>8</v>
-      </c>
-      <c r="G29" s="41"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="56">
+      <c r="C29" s="46"/>
+      <c r="D29" s="40">
+        <v>6</v>
+      </c>
+      <c r="E29" s="39">
+        <v>8</v>
+      </c>
+      <c r="F29" s="36">
+        <v>8</v>
+      </c>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="53">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="36"/>
-      <c r="B30" s="53" t="s">
+    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="76">
+        <v>19702024</v>
+      </c>
+      <c r="B30" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="48">
-        <v>6</v>
-      </c>
-      <c r="D30" s="38">
-        <v>8</v>
-      </c>
-      <c r="E30" s="37">
-        <v>8</v>
-      </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="56">
+      <c r="C30" s="45">
+        <v>6</v>
+      </c>
+      <c r="D30" s="36">
+        <v>8</v>
+      </c>
+      <c r="E30" s="35">
+        <v>8</v>
+      </c>
+      <c r="F30" s="36"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="53">
         <f t="shared" ref="K30:K74" si="1">SUM(C30,D30,E30,F30,G30,H30,I30,J30)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
-      <c r="B31" s="54" t="s">
+    <row r="31" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="76">
+        <v>19702025</v>
+      </c>
+      <c r="B31" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="38">
-        <v>8</v>
-      </c>
-      <c r="E31" s="37">
-        <v>8</v>
-      </c>
-      <c r="F31" s="38">
-        <v>8</v>
-      </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="56">
+      <c r="C31" s="45"/>
+      <c r="D31" s="36">
+        <v>8</v>
+      </c>
+      <c r="E31" s="35">
+        <v>8</v>
+      </c>
+      <c r="F31" s="36">
+        <v>8</v>
+      </c>
+      <c r="G31" s="35"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="53">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="36"/>
-      <c r="B32" s="53" t="s">
+    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="76">
+        <v>19702026</v>
+      </c>
+      <c r="B32" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="48">
-        <v>6</v>
-      </c>
-      <c r="D32" s="38">
-        <v>7</v>
-      </c>
-      <c r="E32" s="37">
-        <v>7</v>
-      </c>
-      <c r="F32" s="38"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="56">
+      <c r="C32" s="45">
+        <v>6</v>
+      </c>
+      <c r="D32" s="36">
+        <v>7</v>
+      </c>
+      <c r="E32" s="35">
+        <v>7</v>
+      </c>
+      <c r="F32" s="36"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="53">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
-      <c r="B33" s="54" t="s">
+    <row r="33" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="76">
+        <v>19702027</v>
+      </c>
+      <c r="B33" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="38">
-        <v>8</v>
-      </c>
-      <c r="E33" s="37">
-        <v>8</v>
-      </c>
-      <c r="F33" s="38">
-        <v>8</v>
-      </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="56">
+      <c r="C33" s="45"/>
+      <c r="D33" s="36">
+        <v>8</v>
+      </c>
+      <c r="E33" s="35">
+        <v>8</v>
+      </c>
+      <c r="F33" s="36">
+        <v>8</v>
+      </c>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="53">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="36"/>
-      <c r="B34" s="53" t="s">
+    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="76">
+        <v>19702028</v>
+      </c>
+      <c r="B34" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="38">
-        <v>8</v>
-      </c>
-      <c r="E34" s="37">
-        <v>8</v>
-      </c>
-      <c r="F34" s="38">
-        <v>8</v>
-      </c>
-      <c r="G34" s="37"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="56">
+      <c r="C34" s="45"/>
+      <c r="D34" s="36">
+        <v>8</v>
+      </c>
+      <c r="E34" s="35">
+        <v>8</v>
+      </c>
+      <c r="F34" s="36">
+        <v>8</v>
+      </c>
+      <c r="G34" s="35"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="53">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
-      <c r="B35" s="54" t="s">
+    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="76">
+        <v>19702029</v>
+      </c>
+      <c r="B35" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="48">
-        <v>7</v>
-      </c>
-      <c r="D35" s="38">
-        <v>7</v>
-      </c>
-      <c r="E35" s="37">
-        <v>6</v>
-      </c>
-      <c r="F35" s="38"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="56">
+      <c r="C35" s="45">
+        <v>7</v>
+      </c>
+      <c r="D35" s="36">
+        <v>7</v>
+      </c>
+      <c r="E35" s="35">
+        <v>6</v>
+      </c>
+      <c r="F35" s="36"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="53">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="36"/>
-      <c r="B36" s="53" t="s">
+    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="76">
+        <v>19702030</v>
+      </c>
+      <c r="B36" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="38">
-        <v>8</v>
-      </c>
-      <c r="E36" s="37">
-        <v>6</v>
-      </c>
-      <c r="F36" s="38">
-        <v>6</v>
-      </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="56">
+      <c r="C36" s="45"/>
+      <c r="D36" s="36">
+        <v>8</v>
+      </c>
+      <c r="E36" s="35">
+        <v>6</v>
+      </c>
+      <c r="F36" s="36">
+        <v>6</v>
+      </c>
+      <c r="G36" s="35"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="53">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
-      <c r="B37" s="54" t="s">
+    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="76">
+        <v>19702031</v>
+      </c>
+      <c r="B37" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="38">
-        <v>8</v>
-      </c>
-      <c r="E37" s="37">
-        <v>7</v>
-      </c>
-      <c r="F37" s="38">
+      <c r="C37" s="45"/>
+      <c r="D37" s="36">
+        <v>8</v>
+      </c>
+      <c r="E37" s="35">
+        <v>7</v>
+      </c>
+      <c r="F37" s="36">
         <v>5</v>
       </c>
-      <c r="G37" s="37"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="56">
+      <c r="G37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="53">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="36"/>
-      <c r="B38" s="53" t="s">
+    <row r="38" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="76">
+        <v>19702032</v>
+      </c>
+      <c r="B38" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="48">
+      <c r="C38" s="45">
         <v>5</v>
       </c>
-      <c r="D38" s="38">
+      <c r="D38" s="36">
         <v>5</v>
       </c>
-      <c r="E38" s="37">
-        <v>6</v>
-      </c>
-      <c r="F38" s="38"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="56">
+      <c r="E38" s="35">
+        <v>6</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="53">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="B39" s="54" t="s">
+    <row r="39" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="76">
+        <v>19702033</v>
+      </c>
+      <c r="B39" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="38">
-        <v>7</v>
-      </c>
-      <c r="E39" s="37">
-        <v>8</v>
-      </c>
-      <c r="F39" s="38">
-        <v>7</v>
-      </c>
-      <c r="G39" s="37"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="56">
+      <c r="C39" s="45"/>
+      <c r="D39" s="36">
+        <v>7</v>
+      </c>
+      <c r="E39" s="35">
+        <v>8</v>
+      </c>
+      <c r="F39" s="36">
+        <v>7</v>
+      </c>
+      <c r="G39" s="35"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="53">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="36"/>
-      <c r="B40" s="53" t="s">
+    <row r="40" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="76">
+        <v>19702034</v>
+      </c>
+      <c r="B40" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="48"/>
-      <c r="D40" s="38">
+      <c r="C40" s="45"/>
+      <c r="D40" s="36">
         <v>5</v>
       </c>
-      <c r="E40" s="37">
-        <v>6</v>
-      </c>
-      <c r="F40" s="38">
+      <c r="E40" s="35">
+        <v>6</v>
+      </c>
+      <c r="F40" s="36">
         <v>5</v>
       </c>
-      <c r="G40" s="37"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="56">
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="37"/>
+      <c r="K40" s="53">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="54" t="s">
+    <row r="41" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="76">
+        <v>19702036</v>
+      </c>
+      <c r="B41" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="48">
+      <c r="C41" s="45">
         <v>4</v>
       </c>
-      <c r="D41" s="38">
-        <v>8</v>
-      </c>
-      <c r="E41" s="37">
-        <v>7</v>
-      </c>
-      <c r="F41" s="38"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="56">
+      <c r="D41" s="36">
+        <v>8</v>
+      </c>
+      <c r="E41" s="35">
+        <v>7</v>
+      </c>
+      <c r="F41" s="36"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="53">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="36"/>
-      <c r="B42" s="53" t="s">
+    <row r="42" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="76">
+        <v>19702037</v>
+      </c>
+      <c r="B42" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="38">
-        <v>6</v>
-      </c>
-      <c r="E42" s="37">
-        <v>7</v>
-      </c>
-      <c r="F42" s="38">
-        <v>7</v>
-      </c>
-      <c r="G42" s="37"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="56">
+      <c r="C42" s="45"/>
+      <c r="D42" s="36">
+        <v>6</v>
+      </c>
+      <c r="E42" s="35">
+        <v>7</v>
+      </c>
+      <c r="F42" s="36">
+        <v>7</v>
+      </c>
+      <c r="G42" s="35"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="53">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="58"/>
-      <c r="B43" s="54" t="s">
+    <row r="43" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="76">
+        <v>19702038</v>
+      </c>
+      <c r="B43" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="49">
-        <v>6</v>
-      </c>
-      <c r="D43" s="42">
-        <v>6</v>
-      </c>
-      <c r="E43" s="41">
-        <v>7</v>
-      </c>
-      <c r="F43" s="42"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="59">
+      <c r="C43" s="46">
+        <v>6</v>
+      </c>
+      <c r="D43" s="40">
+        <v>6</v>
+      </c>
+      <c r="E43" s="39">
+        <v>7</v>
+      </c>
+      <c r="F43" s="40"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="55">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="79"/>
-      <c r="B44" s="53" t="s">
+    <row r="44" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="76">
+        <v>19702039</v>
+      </c>
+      <c r="B44" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="37">
-        <v>6</v>
-      </c>
-      <c r="D44" s="38">
-        <v>7</v>
-      </c>
-      <c r="E44" s="37">
-        <v>7</v>
-      </c>
-      <c r="F44" s="38"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="59">
+      <c r="C44" s="35">
+        <v>6</v>
+      </c>
+      <c r="D44" s="36">
+        <v>7</v>
+      </c>
+      <c r="E44" s="35">
+        <v>7</v>
+      </c>
+      <c r="F44" s="36"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="55">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="79"/>
-      <c r="B45" s="54" t="s">
+    <row r="45" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="76">
+        <v>19702041</v>
+      </c>
+      <c r="B45" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="38">
-        <v>8</v>
-      </c>
-      <c r="E45" s="37">
-        <v>6</v>
-      </c>
-      <c r="F45" s="38">
-        <v>6</v>
-      </c>
-      <c r="G45" s="37"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="59">
+      <c r="C45" s="35"/>
+      <c r="D45" s="36">
+        <v>8</v>
+      </c>
+      <c r="E45" s="35">
+        <v>6</v>
+      </c>
+      <c r="F45" s="36">
+        <v>6</v>
+      </c>
+      <c r="G45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="55">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="79"/>
-      <c r="B46" s="53" t="s">
+    <row r="46" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="76">
+        <v>19702042</v>
+      </c>
+      <c r="B46" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38">
-        <v>8</v>
-      </c>
-      <c r="E46" s="37">
-        <v>8</v>
-      </c>
-      <c r="F46" s="38">
-        <v>8</v>
-      </c>
-      <c r="G46" s="37"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="59">
+      <c r="C46" s="35"/>
+      <c r="D46" s="36">
+        <v>8</v>
+      </c>
+      <c r="E46" s="35">
+        <v>8</v>
+      </c>
+      <c r="F46" s="36">
+        <v>8</v>
+      </c>
+      <c r="G46" s="35"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="55">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="79"/>
-      <c r="B47" s="54" t="s">
+    <row r="47" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="76">
+        <v>19702045</v>
+      </c>
+      <c r="B47" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="38">
-        <v>8</v>
-      </c>
-      <c r="E47" s="37">
-        <v>7</v>
-      </c>
-      <c r="F47" s="38">
-        <v>7</v>
-      </c>
-      <c r="G47" s="37"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="59">
+      <c r="C47" s="35"/>
+      <c r="D47" s="36">
+        <v>8</v>
+      </c>
+      <c r="E47" s="35">
+        <v>7</v>
+      </c>
+      <c r="F47" s="36">
+        <v>7</v>
+      </c>
+      <c r="G47" s="35"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="79"/>
-      <c r="B48" s="53" t="s">
+    <row r="48" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="76">
+        <v>19702046</v>
+      </c>
+      <c r="B48" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="37"/>
-      <c r="D48" s="38">
-        <v>8</v>
-      </c>
-      <c r="E48" s="37">
-        <v>7</v>
-      </c>
-      <c r="F48" s="38">
-        <v>7</v>
-      </c>
-      <c r="G48" s="37"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="59">
+      <c r="C48" s="35"/>
+      <c r="D48" s="36">
+        <v>8</v>
+      </c>
+      <c r="E48" s="35">
+        <v>7</v>
+      </c>
+      <c r="F48" s="36">
+        <v>7</v>
+      </c>
+      <c r="G48" s="35"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="79"/>
-      <c r="B49" s="54" t="s">
+    <row r="49" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="76">
+        <v>19702047</v>
+      </c>
+      <c r="B49" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="37"/>
-      <c r="D49" s="38">
-        <v>7</v>
-      </c>
-      <c r="E49" s="37">
-        <v>7</v>
-      </c>
-      <c r="F49" s="38">
-        <v>7</v>
-      </c>
-      <c r="G49" s="37"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="59">
+      <c r="C49" s="35"/>
+      <c r="D49" s="36">
+        <v>7</v>
+      </c>
+      <c r="E49" s="35">
+        <v>7</v>
+      </c>
+      <c r="F49" s="36">
+        <v>7</v>
+      </c>
+      <c r="G49" s="35"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="79"/>
-      <c r="B50" s="53" t="s">
+    <row r="50" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="76">
+        <v>19702048</v>
+      </c>
+      <c r="B50" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="37">
-        <v>7</v>
-      </c>
-      <c r="D50" s="38">
-        <v>8</v>
-      </c>
-      <c r="E50" s="37">
-        <v>7</v>
-      </c>
-      <c r="F50" s="38"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="59">
+      <c r="C50" s="35">
+        <v>7</v>
+      </c>
+      <c r="D50" s="36">
+        <v>8</v>
+      </c>
+      <c r="E50" s="35">
+        <v>7</v>
+      </c>
+      <c r="F50" s="36"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="79"/>
-      <c r="B51" s="54" t="s">
+    <row r="51" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="76">
+        <v>19702049</v>
+      </c>
+      <c r="B51" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="35">
         <v>4</v>
       </c>
-      <c r="D51" s="38">
-        <v>7</v>
-      </c>
-      <c r="E51" s="37">
-        <v>7</v>
-      </c>
-      <c r="F51" s="38"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="37"/>
-      <c r="K51" s="59">
+      <c r="D51" s="36">
+        <v>7</v>
+      </c>
+      <c r="E51" s="35">
+        <v>7</v>
+      </c>
+      <c r="F51" s="36"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="55">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="79"/>
-      <c r="B52" s="53" t="s">
+    <row r="52" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="76">
+        <v>19702050</v>
+      </c>
+      <c r="B52" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="37"/>
-      <c r="D52" s="38">
-        <v>8</v>
-      </c>
-      <c r="E52" s="37">
-        <v>7</v>
-      </c>
-      <c r="F52" s="38">
-        <v>7</v>
-      </c>
-      <c r="G52" s="37"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
-      <c r="K52" s="59">
+      <c r="C52" s="35"/>
+      <c r="D52" s="36">
+        <v>8</v>
+      </c>
+      <c r="E52" s="35">
+        <v>7</v>
+      </c>
+      <c r="F52" s="36">
+        <v>7</v>
+      </c>
+      <c r="G52" s="35"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="79"/>
-      <c r="B53" s="54" t="s">
+    <row r="53" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="76">
+        <v>19702051</v>
+      </c>
+      <c r="B53" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="37"/>
-      <c r="D53" s="38">
-        <v>7</v>
-      </c>
-      <c r="E53" s="37">
-        <v>7</v>
-      </c>
-      <c r="F53" s="38">
-        <v>7</v>
-      </c>
-      <c r="G53" s="37"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="59">
+      <c r="C53" s="35"/>
+      <c r="D53" s="36">
+        <v>7</v>
+      </c>
+      <c r="E53" s="35">
+        <v>7</v>
+      </c>
+      <c r="F53" s="36">
+        <v>7</v>
+      </c>
+      <c r="G53" s="35"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="79"/>
-      <c r="B54" s="53" t="s">
+    <row r="54" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="76">
+        <v>19702052</v>
+      </c>
+      <c r="B54" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="38">
-        <v>8</v>
-      </c>
-      <c r="E54" s="37">
-        <v>7</v>
-      </c>
-      <c r="F54" s="38">
-        <v>6</v>
-      </c>
-      <c r="G54" s="37"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="59">
+      <c r="C54" s="35"/>
+      <c r="D54" s="36">
+        <v>8</v>
+      </c>
+      <c r="E54" s="35">
+        <v>7</v>
+      </c>
+      <c r="F54" s="36">
+        <v>6</v>
+      </c>
+      <c r="G54" s="35"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="79"/>
-      <c r="B55" s="54" t="s">
+    <row r="55" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="76">
+        <v>19702053</v>
+      </c>
+      <c r="B55" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="37"/>
-      <c r="D55" s="38">
-        <v>8</v>
-      </c>
-      <c r="E55" s="37">
-        <v>7</v>
-      </c>
-      <c r="F55" s="38">
-        <v>7</v>
-      </c>
-      <c r="G55" s="37"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="59">
+      <c r="C55" s="35"/>
+      <c r="D55" s="36">
+        <v>8</v>
+      </c>
+      <c r="E55" s="35">
+        <v>7</v>
+      </c>
+      <c r="F55" s="36">
+        <v>7</v>
+      </c>
+      <c r="G55" s="35"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="79"/>
-      <c r="B56" s="53" t="s">
+    <row r="56" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="76">
+        <v>19702054</v>
+      </c>
+      <c r="B56" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="37">
+      <c r="C56" s="35">
         <v>5</v>
       </c>
-      <c r="D56" s="38">
-        <v>8</v>
-      </c>
-      <c r="E56" s="37">
-        <v>7</v>
-      </c>
-      <c r="F56" s="38"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="38"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
-      <c r="K56" s="59">
+      <c r="D56" s="36">
+        <v>8</v>
+      </c>
+      <c r="E56" s="35">
+        <v>7</v>
+      </c>
+      <c r="F56" s="36"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="55">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="79"/>
-      <c r="B57" s="54" t="s">
+    <row r="57" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="76">
+        <v>19702055</v>
+      </c>
+      <c r="B57" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="37"/>
-      <c r="D57" s="38">
-        <v>8</v>
-      </c>
-      <c r="E57" s="37">
-        <v>8</v>
-      </c>
-      <c r="F57" s="38">
-        <v>8</v>
-      </c>
-      <c r="G57" s="37"/>
-      <c r="H57" s="38"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="59">
+      <c r="C57" s="35"/>
+      <c r="D57" s="36">
+        <v>8</v>
+      </c>
+      <c r="E57" s="35">
+        <v>8</v>
+      </c>
+      <c r="F57" s="36">
+        <v>8</v>
+      </c>
+      <c r="G57" s="35"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="55">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="79"/>
-      <c r="B58" s="53" t="s">
+    <row r="58" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="76">
+        <v>19702056</v>
+      </c>
+      <c r="B58" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="37"/>
-      <c r="D58" s="38">
+      <c r="C58" s="35"/>
+      <c r="D58" s="36">
         <v>5</v>
       </c>
-      <c r="E58" s="37">
-        <v>7</v>
-      </c>
-      <c r="F58" s="38">
-        <v>6</v>
-      </c>
-      <c r="G58" s="37"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="59">
+      <c r="E58" s="35">
+        <v>7</v>
+      </c>
+      <c r="F58" s="36">
+        <v>6</v>
+      </c>
+      <c r="G58" s="35"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="55">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="79"/>
-      <c r="B59" s="54" t="s">
+    <row r="59" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="76">
+        <v>19702057</v>
+      </c>
+      <c r="B59" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="37"/>
-      <c r="D59" s="38">
-        <v>7</v>
-      </c>
-      <c r="E59" s="37">
-        <v>7</v>
-      </c>
-      <c r="F59" s="38">
-        <v>8</v>
-      </c>
-      <c r="G59" s="37"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="59">
+      <c r="C59" s="35"/>
+      <c r="D59" s="36">
+        <v>7</v>
+      </c>
+      <c r="E59" s="35">
+        <v>7</v>
+      </c>
+      <c r="F59" s="36">
+        <v>8</v>
+      </c>
+      <c r="G59" s="35"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="79"/>
-      <c r="B60" s="53" t="s">
+    <row r="60" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="76">
+        <v>19702059</v>
+      </c>
+      <c r="B60" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="37">
-        <v>6</v>
-      </c>
-      <c r="D60" s="38">
-        <v>8</v>
-      </c>
-      <c r="E60" s="37">
-        <v>7</v>
-      </c>
-      <c r="F60" s="38"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="59">
+      <c r="C60" s="35">
+        <v>6</v>
+      </c>
+      <c r="D60" s="36">
+        <v>8</v>
+      </c>
+      <c r="E60" s="35">
+        <v>7</v>
+      </c>
+      <c r="F60" s="36"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="79"/>
-      <c r="B61" s="54" t="s">
+    <row r="61" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="76">
+        <v>19702060</v>
+      </c>
+      <c r="B61" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="38">
+      <c r="C61" s="36">
         <v>3</v>
       </c>
-      <c r="D61" s="38">
-        <v>8</v>
-      </c>
-      <c r="E61" s="37">
-        <v>7</v>
-      </c>
-      <c r="F61" s="38"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="38"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="59">
+      <c r="D61" s="36">
+        <v>8</v>
+      </c>
+      <c r="E61" s="35">
+        <v>7</v>
+      </c>
+      <c r="F61" s="36"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="36"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="55">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="79"/>
-      <c r="B62" s="53" t="s">
+    <row r="62" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="76">
+        <v>19702061</v>
+      </c>
+      <c r="B62" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="37"/>
-      <c r="D62" s="38">
-        <v>8</v>
-      </c>
-      <c r="E62" s="37">
-        <v>7</v>
-      </c>
-      <c r="F62" s="38">
-        <v>6</v>
-      </c>
-      <c r="G62" s="37"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="59">
+      <c r="C62" s="35"/>
+      <c r="D62" s="36">
+        <v>8</v>
+      </c>
+      <c r="E62" s="35">
+        <v>7</v>
+      </c>
+      <c r="F62" s="36">
+        <v>6</v>
+      </c>
+      <c r="G62" s="35"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="79"/>
-      <c r="B63" s="54" t="s">
+    <row r="63" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="76">
+        <v>19702062</v>
+      </c>
+      <c r="B63" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C63" s="37">
-        <v>6</v>
-      </c>
-      <c r="D63" s="38">
-        <v>7</v>
-      </c>
-      <c r="E63" s="37">
-        <v>8</v>
-      </c>
-      <c r="F63" s="38"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="59">
+      <c r="C63" s="35">
+        <v>6</v>
+      </c>
+      <c r="D63" s="36">
+        <v>7</v>
+      </c>
+      <c r="E63" s="35">
+        <v>8</v>
+      </c>
+      <c r="F63" s="36"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="36"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="79"/>
-      <c r="B64" s="53" t="s">
+    <row r="64" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="76">
+        <v>19702064</v>
+      </c>
+      <c r="B64" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="37"/>
-      <c r="D64" s="38">
-        <v>8</v>
-      </c>
-      <c r="E64" s="37">
-        <v>8</v>
-      </c>
-      <c r="F64" s="38">
-        <v>7</v>
-      </c>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="37"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="59">
+      <c r="C64" s="35"/>
+      <c r="D64" s="36">
+        <v>8</v>
+      </c>
+      <c r="E64" s="35">
+        <v>8</v>
+      </c>
+      <c r="F64" s="36">
+        <v>7</v>
+      </c>
+      <c r="G64" s="35"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="55">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="79"/>
-      <c r="B65" s="54" t="s">
+    <row r="65" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="76">
+        <v>19702065</v>
+      </c>
+      <c r="B65" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="37">
-        <v>6</v>
-      </c>
-      <c r="D65" s="38">
-        <v>8</v>
-      </c>
-      <c r="E65" s="37"/>
-      <c r="F65" s="38">
-        <v>8</v>
-      </c>
-      <c r="G65" s="37"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="37"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="59">
+      <c r="C65" s="35">
+        <v>6</v>
+      </c>
+      <c r="D65" s="36">
+        <v>8</v>
+      </c>
+      <c r="E65" s="35"/>
+      <c r="F65" s="36">
+        <v>8</v>
+      </c>
+      <c r="G65" s="35"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="79"/>
-      <c r="B66" s="53" t="s">
+    <row r="66" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="76">
+        <v>18702006</v>
+      </c>
+      <c r="B66" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="38">
-        <v>6</v>
-      </c>
-      <c r="E66" s="37">
-        <v>8</v>
-      </c>
-      <c r="F66" s="38">
-        <v>7</v>
-      </c>
-      <c r="G66" s="37"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="37"/>
-      <c r="J66" s="37"/>
-      <c r="K66" s="59">
+      <c r="C66" s="35"/>
+      <c r="D66" s="36">
+        <v>6</v>
+      </c>
+      <c r="E66" s="35">
+        <v>8</v>
+      </c>
+      <c r="F66" s="36">
+        <v>7</v>
+      </c>
+      <c r="G66" s="35"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="79"/>
-      <c r="B67" s="54" t="s">
+    <row r="67" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="76">
+        <v>18702008</v>
+      </c>
+      <c r="B67" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="38">
+      <c r="C67" s="35"/>
+      <c r="D67" s="36">
         <v>5</v>
       </c>
-      <c r="E67" s="37">
-        <v>6</v>
-      </c>
-      <c r="F67" s="38">
+      <c r="E67" s="35">
+        <v>6</v>
+      </c>
+      <c r="F67" s="36">
         <v>5</v>
       </c>
-      <c r="G67" s="37"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="59">
+      <c r="G67" s="35"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="55">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="79"/>
-      <c r="B68" s="53" t="s">
+    <row r="68" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="76">
+        <v>18702016</v>
+      </c>
+      <c r="B68" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="37"/>
-      <c r="D68" s="38">
-        <v>8</v>
-      </c>
-      <c r="E68" s="37">
-        <v>7</v>
-      </c>
-      <c r="F68" s="38">
-        <v>6</v>
-      </c>
-      <c r="G68" s="37"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="37"/>
-      <c r="J68" s="37"/>
-      <c r="K68" s="59">
+      <c r="C68" s="35"/>
+      <c r="D68" s="36">
+        <v>8</v>
+      </c>
+      <c r="E68" s="35">
+        <v>7</v>
+      </c>
+      <c r="F68" s="36">
+        <v>6</v>
+      </c>
+      <c r="G68" s="35"/>
+      <c r="H68" s="36"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="55">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="79"/>
-      <c r="B69" s="54" t="s">
+    <row r="69" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="76">
+        <v>18702032</v>
+      </c>
+      <c r="B69" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="37">
-        <v>7</v>
-      </c>
-      <c r="D69" s="38">
-        <v>8</v>
-      </c>
-      <c r="E69" s="37">
-        <v>8</v>
-      </c>
-      <c r="F69" s="38"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="37"/>
-      <c r="J69" s="37"/>
-      <c r="K69" s="59">
+      <c r="C69" s="35">
+        <v>7</v>
+      </c>
+      <c r="D69" s="36">
+        <v>8</v>
+      </c>
+      <c r="E69" s="35">
+        <v>8</v>
+      </c>
+      <c r="F69" s="36"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="55">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="79"/>
-      <c r="B70" s="53" t="s">
+    <row r="70" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="76">
+        <v>18702037</v>
+      </c>
+      <c r="B70" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="37">
-        <v>7</v>
-      </c>
-      <c r="D70" s="38">
-        <v>8</v>
-      </c>
-      <c r="E70" s="37"/>
-      <c r="F70" s="38">
-        <v>7</v>
-      </c>
-      <c r="G70" s="37"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="37"/>
-      <c r="J70" s="37"/>
-      <c r="K70" s="59">
+      <c r="C70" s="35">
+        <v>7</v>
+      </c>
+      <c r="D70" s="36">
+        <v>8</v>
+      </c>
+      <c r="E70" s="35"/>
+      <c r="F70" s="36">
+        <v>7</v>
+      </c>
+      <c r="G70" s="35"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="35"/>
+      <c r="J70" s="35"/>
+      <c r="K70" s="55">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="79"/>
-      <c r="B71" s="54" t="s">
+    <row r="71" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="76">
+        <v>18702043</v>
+      </c>
+      <c r="B71" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C71" s="37">
-        <v>6</v>
-      </c>
-      <c r="D71" s="38"/>
-      <c r="E71" s="37">
-        <v>7</v>
-      </c>
-      <c r="F71" s="38">
-        <v>7</v>
-      </c>
-      <c r="G71" s="37"/>
-      <c r="H71" s="38"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="37"/>
-      <c r="K71" s="59">
+      <c r="C71" s="35">
+        <v>6</v>
+      </c>
+      <c r="D71" s="36"/>
+      <c r="E71" s="35">
+        <v>7</v>
+      </c>
+      <c r="F71" s="36">
+        <v>7</v>
+      </c>
+      <c r="G71" s="35"/>
+      <c r="H71" s="36"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="35"/>
+      <c r="K71" s="55">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="79"/>
-      <c r="B72" s="53" t="s">
+    <row r="72" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="76">
+        <v>18702046</v>
+      </c>
+      <c r="B72" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="C72" s="37">
+      <c r="C72" s="35">
         <v>5</v>
       </c>
-      <c r="D72" s="38">
-        <v>7</v>
-      </c>
-      <c r="E72" s="37">
-        <v>7</v>
-      </c>
-      <c r="F72" s="38"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="37"/>
-      <c r="J72" s="37"/>
-      <c r="K72" s="59">
+      <c r="D72" s="36">
+        <v>7</v>
+      </c>
+      <c r="E72" s="35">
+        <v>7</v>
+      </c>
+      <c r="F72" s="36"/>
+      <c r="G72" s="35"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="55">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="79"/>
-      <c r="B73" s="54" t="s">
+    <row r="73" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="76">
+        <v>18702047</v>
+      </c>
+      <c r="B73" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="37">
+      <c r="C73" s="35">
         <v>5</v>
       </c>
-      <c r="D73" s="38">
-        <v>6</v>
-      </c>
-      <c r="E73" s="37">
-        <v>7</v>
-      </c>
-      <c r="F73" s="38"/>
-      <c r="G73" s="37"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="37"/>
-      <c r="J73" s="37"/>
-      <c r="K73" s="59">
+      <c r="D73" s="36">
+        <v>6</v>
+      </c>
+      <c r="E73" s="35">
+        <v>7</v>
+      </c>
+      <c r="F73" s="36"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="35"/>
+      <c r="J73" s="35"/>
+      <c r="K73" s="55">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="80"/>
-      <c r="B74" s="81" t="s">
+    <row r="74" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="76">
+        <v>18702050</v>
+      </c>
+      <c r="B74" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C74" s="45">
+      <c r="C74" s="42">
         <v>4</v>
       </c>
-      <c r="D74" s="46">
-        <v>6</v>
-      </c>
-      <c r="E74" s="45">
-        <v>6</v>
-      </c>
-      <c r="F74" s="46"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="46"/>
-      <c r="I74" s="45"/>
-      <c r="J74" s="45"/>
-      <c r="K74" s="57">
+      <c r="D74" s="43">
+        <v>6</v>
+      </c>
+      <c r="E74" s="42">
+        <v>6</v>
+      </c>
+      <c r="F74" s="43"/>
+      <c r="G74" s="42"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="42"/>
+      <c r="J74" s="42"/>
+      <c r="K74" s="54">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="27"/>
-      <c r="B75" s="52"/>
+    <row r="75" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="76">
+        <v>18702053</v>
+      </c>
+      <c r="B75" s="49"/>
       <c r="C75" s="27"/>
       <c r="D75" s="29"/>
       <c r="E75" s="27"/>
@@ -3317,79 +3398,97 @@
       <c r="H75" s="29"/>
       <c r="I75" s="27"/>
       <c r="J75" s="27"/>
-      <c r="K75" s="52"/>
-    </row>
-    <row r="76" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K75" s="49"/>
+    </row>
+    <row r="76" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="76">
+        <v>18702057</v>
+      </c>
       <c r="D76" s="28"/>
       <c r="F76" s="28"/>
       <c r="H76" s="28"/>
     </row>
-    <row r="77" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="76">
+        <v>18702059</v>
+      </c>
       <c r="D77" s="28"/>
       <c r="F77" s="28"/>
       <c r="H77" s="28"/>
     </row>
-    <row r="78" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="76">
+        <v>18702063</v>
+      </c>
       <c r="D78" s="28"/>
       <c r="F78" s="28"/>
       <c r="H78" s="28"/>
     </row>
-    <row r="79" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="76">
+        <v>18702066</v>
+      </c>
       <c r="D79" s="28"/>
       <c r="F79" s="28"/>
       <c r="H79" s="28"/>
     </row>
-    <row r="80" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="76">
+        <v>18702068</v>
+      </c>
       <c r="D80" s="28"/>
       <c r="F80" s="28"/>
       <c r="H80" s="28"/>
     </row>
-    <row r="81" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="76">
+        <v>16702055</v>
+      </c>
       <c r="D81" s="28"/>
       <c r="F81" s="28"/>
       <c r="H81" s="28"/>
     </row>
-    <row r="82" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D82" s="28"/>
       <c r="F82" s="28"/>
       <c r="H82" s="28"/>
     </row>
-    <row r="83" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D83" s="28"/>
       <c r="F83" s="28"/>
       <c r="H83" s="28"/>
     </row>
-    <row r="84" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D84" s="28"/>
       <c r="F84" s="28"/>
       <c r="H84" s="28"/>
     </row>
-    <row r="85" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D85" s="28"/>
       <c r="F85" s="28"/>
       <c r="H85" s="28"/>
     </row>
-    <row r="86" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D86" s="28"/>
       <c r="F86" s="28"/>
       <c r="H86" s="28"/>
     </row>
-    <row r="87" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D87" s="28"/>
       <c r="F87" s="28"/>
       <c r="H87" s="28"/>
     </row>
-    <row r="88" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D88" s="28"/>
       <c r="F88" s="28"/>
       <c r="H88" s="28"/>
     </row>
-    <row r="89" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D89" s="28"/>
       <c r="F89" s="28"/>
       <c r="H89" s="28"/>
     </row>
-    <row r="90" spans="4:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D90" s="28"/>
       <c r="F90" s="28"/>
       <c r="H90" s="28"/>
@@ -3417,7 +3516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:K49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -3429,79 +3528,79 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A6" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="A6" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
     </row>
     <row r="9" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
@@ -3510,10 +3609,10 @@
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="68"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -3735,94 +3834,94 @@
       <c r="K21" s="10"/>
     </row>
     <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A34" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
+      <c r="A34" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
     </row>
     <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A35" s="78" t="s">
+      <c r="A35" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="66"/>
     </row>
     <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
     </row>
     <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="65"/>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A38" s="68" t="s">
+      <c r="A38" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.15">
-      <c r="A39" s="68" t="s">
+      <c r="A39" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="68"/>
-      <c r="H39" s="68"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="68"/>
-      <c r="K39" s="68"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="65"/>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
@@ -3851,42 +3950,42 @@
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A42" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="72" t="s">
+      <c r="A42" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="73"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="69" t="s">
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="67" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="70"/>
-      <c r="B43" s="70"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="70"/>
+      <c r="A43" s="68"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="68"/>
     </row>
     <row r="44" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="71"/>
-      <c r="B44" s="71"/>
+      <c r="A44" s="69"/>
+      <c r="B44" s="69"/>
       <c r="C44" s="5">
         <v>1</v>
       </c>
@@ -3911,7 +4010,7 @@
       <c r="J44" s="7">
         <v>8</v>
       </c>
-      <c r="K44" s="71"/>
+      <c r="K44" s="69"/>
     </row>
     <row r="45" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
@@ -4040,6 +4139,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:J43"/>
+    <mergeCell ref="K42:K44"/>
     <mergeCell ref="A34:K34"/>
     <mergeCell ref="A35:K35"/>
     <mergeCell ref="E11:F11"/>
@@ -4048,14 +4155,6 @@
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A9:K9"/>
     <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:J43"/>
-    <mergeCell ref="K42:K44"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.74685039370078743" right="0.16" top="0.6100000000000001" bottom="0" header="0.31" footer="0"/>

</xml_diff>